<commit_message>
Muchos cambios para que funcione el BottonNavigationBar :(
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\Desktop\Flutter\udd_bootcamp\proyecto_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F3829E3-F642-49B4-93A1-39C57DE0838C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CC548E-DA51-491A-99AF-8A658B49AFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{163A0881-EA6B-414E-ABC8-390A3BF5A502}"/>
   </bookViews>
@@ -187,9 +187,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -197,13 +194,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0623C1-D010-4467-B8E6-B15EB88880C5}">
   <dimension ref="B3:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,137 +546,137 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="45" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="45" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="B7" s="6"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="B9" s="6"/>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3" t="s">
+    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.3">
+      <c r="B11" s="7"/>
+      <c r="C11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>